<commit_message>
Published state of ETDataset on 13 November 2015
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_regasification_lng.converter.xlsx
+++ b/nodes_source_analyses/energy/energy_regasification_lng.converter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="762" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23460" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="121">
   <si>
     <t>Source</t>
   </si>
@@ -405,12 +405,6 @@
   </si>
   <si>
     <t>Page</t>
-  </si>
-  <si>
-    <t>Set output LNG</t>
-  </si>
-  <si>
-    <t>Set to 1 due to initialisation constraints</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1235,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1326,9 +1320,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
@@ -1468,6 +1459,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="26" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="29" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1504,7 +1496,6 @@
     <xf numFmtId="0" fontId="29" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="273">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2564,105 +2555,105 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1"/>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="94"/>
+      <c r="C9" s="93"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="96"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="95"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1"/>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="96" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="95"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" thickBot="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="98" t="s">
+      <c r="B13" s="94"/>
+      <c r="C13" s="97" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="96" t="s">
+      <c r="B14" s="94"/>
+      <c r="C14" s="95" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="96"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="95"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1"/>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="C16" s="98" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="100" t="s">
+      <c r="B17" s="94"/>
+      <c r="C17" s="99" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="101" t="s">
+      <c r="B18" s="94"/>
+      <c r="C18" s="100" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="102" t="s">
+      <c r="B19" s="94"/>
+      <c r="C19" s="101" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="104" t="s">
+      <c r="B20" s="102"/>
+      <c r="C20" s="103" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="105" t="s">
+      <c r="B21" s="102"/>
+      <c r="C21" s="104" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1"/>
-      <c r="B22" s="103"/>
-      <c r="C22" s="106" t="s">
+      <c r="B22" s="102"/>
+      <c r="C22" s="105" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="103"/>
-      <c r="C23" s="107" t="s">
+      <c r="B23" s="102"/>
+      <c r="C23" s="106" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2684,7 +2675,7 @@
   </sheetPr>
   <dimension ref="B1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -2780,7 +2771,7 @@
       <c r="I9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="114"/>
+      <c r="J9" s="113"/>
     </row>
     <row r="10" spans="2:11" s="26" customFormat="1">
       <c r="B10" s="25"/>
@@ -2808,22 +2799,22 @@
     </row>
     <row r="12" spans="2:11" s="26" customFormat="1" ht="16" thickBot="1">
       <c r="B12" s="25"/>
-      <c r="C12" s="128" t="s">
+      <c r="C12" s="127" t="s">
         <v>64</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="134">
+      <c r="E12" s="133">
         <f>'Research data'!H7</f>
-        <v>1</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="F12" s="40"/>
-      <c r="G12" s="128" t="s">
+      <c r="G12" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H12" s="32"/>
-      <c r="I12" s="148" t="s">
+      <c r="I12" s="147" t="s">
         <v>117</v>
       </c>
       <c r="J12" s="14"/>
@@ -2837,7 +2828,7 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
-      <c r="J13" s="115"/>
+      <c r="J13" s="114"/>
       <c r="K13" s="37"/>
     </row>
     <row r="14" spans="2:11" ht="16" thickBot="1">
@@ -2851,7 +2842,7 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
-      <c r="J14" s="115"/>
+      <c r="J14" s="114"/>
       <c r="K14" s="37"/>
     </row>
     <row r="15" spans="2:11" ht="16" thickBot="1">
@@ -2871,10 +2862,10 @@
         <v>6</v>
       </c>
       <c r="H15" s="40"/>
-      <c r="I15" s="148" t="s">
+      <c r="I15" s="147" t="s">
         <v>116</v>
       </c>
-      <c r="J15" s="115"/>
+      <c r="J15" s="114"/>
     </row>
     <row r="16" spans="2:11" ht="16" thickBot="1">
       <c r="B16" s="41"/>
@@ -2884,7 +2875,7 @@
       <c r="D16" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="113">
+      <c r="E16" s="112">
         <f>'Research data'!L11</f>
         <v>40252688.618643649</v>
       </c>
@@ -2893,56 +2884,56 @@
         <v>26</v>
       </c>
       <c r="H16" s="40"/>
-      <c r="I16" s="148" t="s">
+      <c r="I16" s="147" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="115"/>
+      <c r="J16" s="114"/>
     </row>
     <row r="17" spans="2:10" ht="16" thickBot="1">
       <c r="B17" s="41"/>
-      <c r="C17" s="145" t="s">
+      <c r="C17" s="144" t="s">
         <v>113</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="153">
+      <c r="E17" s="152">
         <f>'Research data'!H12</f>
         <v>1.1261202185792348E-4</v>
       </c>
       <c r="F17" s="40"/>
-      <c r="G17" s="145" t="s">
+      <c r="G17" s="144" t="s">
         <v>111</v>
       </c>
       <c r="H17" s="40"/>
-      <c r="I17" s="148" t="s">
+      <c r="I17" s="147" t="s">
         <v>112</v>
       </c>
-      <c r="J17" s="115"/>
+      <c r="J17" s="114"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="41"/>
       <c r="C18" s="37"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="117"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="116"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="115"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="114"/>
     </row>
     <row r="19" spans="2:10" ht="16" thickBot="1">
       <c r="B19" s="41"/>
       <c r="C19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="116"/>
-      <c r="E19" s="117"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="116"/>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="115"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="114"/>
     </row>
     <row r="20" spans="2:10" ht="16" thickBot="1">
       <c r="B20" s="41"/>
@@ -2957,14 +2948,14 @@
         <v>40</v>
       </c>
       <c r="F20" s="40"/>
-      <c r="G20" s="91" t="s">
+      <c r="G20" s="90" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="40"/>
-      <c r="I20" s="130" t="s">
+      <c r="I20" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="115"/>
+      <c r="J20" s="114"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" thickBot="1">
       <c r="B21" s="41"/>
@@ -2981,7 +2972,7 @@
       <c r="G21" s="40"/>
       <c r="H21" s="40"/>
       <c r="I21" s="35"/>
-      <c r="J21" s="115"/>
+      <c r="J21" s="114"/>
     </row>
     <row r="22" spans="2:10" ht="16" thickBot="1">
       <c r="B22" s="43"/>
@@ -3047,8 +3038,8 @@
   </sheetPr>
   <dimension ref="B2:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3100,40 +3091,33 @@
     </row>
     <row r="4" spans="2:20" s="26" customFormat="1">
       <c r="B4" s="25"/>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="108" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="109" t="s">
+      <c r="F4" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109" t="s">
+      <c r="G4" s="108"/>
+      <c r="H4" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109" t="s">
+      <c r="I4" s="108"/>
+      <c r="J4" s="108" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109" t="s">
+      <c r="K4" s="108"/>
+      <c r="L4" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="109"/>
-      <c r="N4" s="109" t="s">
+      <c r="M4" s="108"/>
+      <c r="N4" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="109"/>
-      <c r="P4" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="109"/>
-      <c r="R4" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="109"/>
-      <c r="T4" s="109" t="s">
+      <c r="O4" s="108"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="108" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3151,8 +3135,7 @@
       <c r="L5" s="54"/>
       <c r="M5" s="54"/>
       <c r="N5" s="56"/>
-      <c r="R5" s="50"/>
-      <c r="T5" s="65"/>
+      <c r="Q5" s="64"/>
     </row>
     <row r="6" spans="2:20" ht="18" customHeight="1" thickBot="1">
       <c r="B6" s="49"/>
@@ -3172,46 +3155,35 @@
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
       <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
-      <c r="T6" s="63"/>
+      <c r="Q6" s="62"/>
     </row>
     <row r="7" spans="2:20" ht="16" thickBot="1">
       <c r="B7" s="49"/>
-      <c r="C7" s="129" t="s">
+      <c r="C7" s="128" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="58"/>
       <c r="E7" s="58"/>
-      <c r="F7" s="131" t="s">
+      <c r="F7" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="110"/>
-      <c r="H7" s="133">
+      <c r="G7" s="109"/>
+      <c r="H7" s="132">
         <f>J7</f>
-        <v>1</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="I7" s="54"/>
-      <c r="J7" s="133">
-        <f>Notes!E48</f>
-        <v>1</v>
+      <c r="J7" s="132">
+        <f>Notes!E47</f>
+        <v>0.98499999999999999</v>
       </c>
       <c r="K7" s="54"/>
-      <c r="L7" s="64"/>
+      <c r="L7" s="63"/>
       <c r="M7" s="54"/>
-      <c r="N7" s="64"/>
+      <c r="N7" s="63"/>
       <c r="O7" s="50"/>
-      <c r="P7" s="59">
-        <f>Notes!$E$46</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="166" t="s">
-        <v>122</v>
-      </c>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="153"/>
     </row>
     <row r="8" spans="2:20">
       <c r="B8" s="49"/>
@@ -3219,20 +3191,17 @@
       <c r="D8" s="58"/>
       <c r="E8" s="58"/>
       <c r="F8" s="52"/>
-      <c r="G8" s="110"/>
-      <c r="H8" s="64"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="63"/>
       <c r="I8" s="54"/>
       <c r="J8" s="54"/>
       <c r="K8" s="54"/>
-      <c r="L8" s="64"/>
+      <c r="L8" s="63"/>
       <c r="M8" s="54"/>
-      <c r="N8" s="64"/>
+      <c r="N8" s="63"/>
       <c r="O8" s="50"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="69"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="68"/>
     </row>
     <row r="9" spans="2:20" ht="16" thickBot="1">
       <c r="B9" s="49"/>
@@ -3252,145 +3221,130 @@
       <c r="N9" s="50"/>
       <c r="O9" s="50"/>
       <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="69"/>
+      <c r="Q9" s="68"/>
     </row>
     <row r="10" spans="2:20" ht="16" thickBot="1">
       <c r="B10" s="49"/>
-      <c r="C10" s="150" t="s">
+      <c r="C10" s="149" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="111"/>
+      <c r="G10" s="110"/>
       <c r="H10" s="55">
         <f>N10</f>
         <v>1090000000</v>
       </c>
       <c r="I10" s="11"/>
-      <c r="K10" s="67"/>
-      <c r="M10" s="67"/>
+      <c r="K10" s="66"/>
+      <c r="M10" s="66"/>
       <c r="N10" s="55">
         <f>Notes!E19+Notes!E13</f>
         <v>1090000000</v>
       </c>
       <c r="O10" s="50"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="137" t="s">
+      <c r="P10" s="50"/>
+      <c r="Q10" s="136" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:20" ht="16" thickBot="1">
       <c r="B11" s="49"/>
-      <c r="C11" s="150" t="s">
+      <c r="C11" s="149" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="108" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="112"/>
+      <c r="G11" s="111"/>
       <c r="H11" s="55">
         <f>L11</f>
         <v>40252688.618643649</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="K11" s="62"/>
+      <c r="I11" s="61"/>
+      <c r="K11" s="61"/>
       <c r="L11" s="55">
         <f>Notes!E73</f>
         <v>40252688.618643649</v>
       </c>
-      <c r="M11" s="62"/>
+      <c r="M11" s="61"/>
       <c r="N11" s="50"/>
       <c r="O11" s="50"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="55">
-        <f>Notes!E39</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="50"/>
-      <c r="T11" s="53"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="53"/>
     </row>
     <row r="12" spans="2:20" ht="16" thickBot="1">
       <c r="B12" s="49"/>
-      <c r="C12" s="150" t="s">
+      <c r="C12" s="149" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="151" t="s">
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="112"/>
-      <c r="H12" s="152">
+      <c r="G12" s="111"/>
+      <c r="H12" s="151">
         <f>L12</f>
         <v>1.1261202185792348E-4</v>
       </c>
-      <c r="I12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="152">
+      <c r="I12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="151">
         <f>Notes!E80</f>
         <v>1.1261202185792348E-4</v>
       </c>
-      <c r="M12" s="62"/>
+      <c r="M12" s="61"/>
       <c r="N12" s="50"/>
       <c r="O12" s="50"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="137" t="s">
+      <c r="P12" s="50"/>
+      <c r="Q12" s="136" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" spans="2:20">
       <c r="B13" s="49"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="65"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="64"/>
     </row>
     <row r="14" spans="2:20" ht="16" thickBot="1">
       <c r="B14" s="49"/>
       <c r="C14" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="S14" s="54"/>
-      <c r="T14" s="68"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="67"/>
     </row>
     <row r="15" spans="2:20" ht="16" thickBot="1">
       <c r="B15" s="49"/>
-      <c r="C15" s="129" t="s">
+      <c r="C15" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="132" t="s">
+      <c r="F15" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="60">
         <f>L15</f>
         <v>40</v>
       </c>
-      <c r="L15" s="61">
+      <c r="L15" s="60">
         <f>Notes!E33</f>
         <v>40</v>
       </c>
-      <c r="S15" s="54"/>
-      <c r="T15" s="69"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="68"/>
     </row>
     <row r="16" spans="2:20" ht="16" thickBot="1">
-      <c r="C16" s="129" t="s">
+      <c r="C16" s="128" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="12"/>
-      <c r="H16" s="61"/>
+      <c r="H16" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3416,32 +3370,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="71" customWidth="1"/>
-    <col min="2" max="2" width="6.375" style="71" customWidth="1"/>
-    <col min="3" max="3" width="27.875" style="71" customWidth="1"/>
-    <col min="4" max="4" width="16.125" style="71" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="71" customWidth="1"/>
-    <col min="6" max="7" width="13.125" style="71" customWidth="1"/>
-    <col min="8" max="8" width="12.625" style="76" customWidth="1"/>
-    <col min="9" max="9" width="31.5" style="76" customWidth="1"/>
-    <col min="10" max="10" width="98.375" style="71" customWidth="1"/>
-    <col min="11" max="16384" width="33.125" style="71"/>
+    <col min="1" max="1" width="3.5" style="70" customWidth="1"/>
+    <col min="2" max="2" width="6.375" style="70" customWidth="1"/>
+    <col min="3" max="3" width="27.875" style="70" customWidth="1"/>
+    <col min="4" max="4" width="16.125" style="70" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="70" customWidth="1"/>
+    <col min="6" max="7" width="13.125" style="70" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="75" customWidth="1"/>
+    <col min="9" max="9" width="31.5" style="75" customWidth="1"/>
+    <col min="10" max="10" width="98.375" style="70" customWidth="1"/>
+    <col min="11" max="16384" width="33.125" style="70"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="16" thickBot="1"/>
     <row r="2" spans="2:10">
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="73"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="72"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="74"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="13" t="s">
         <v>15</v>
       </c>
@@ -3451,21 +3405,21 @@
       <c r="G3" s="13"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
-      <c r="J3" s="70"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="74"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="70"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="79"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="15" t="s">
         <v>16</v>
       </c>
@@ -3492,7 +3446,7 @@
       </c>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="74"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -3503,26 +3457,26 @@
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="74"/>
-      <c r="C7" s="80" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="126" t="s">
+      <c r="D7" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="69">
         <v>2012</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7" s="69">
         <v>2012</v>
       </c>
-      <c r="H7" s="127">
+      <c r="H7" s="126">
         <v>42278</v>
       </c>
-      <c r="I7" s="122" t="s">
+      <c r="I7" s="121" t="s">
         <v>75</v>
       </c>
       <c r="J7" s="51" t="s">
@@ -3530,171 +3484,171 @@
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="74"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="74"/>
-      <c r="C9" s="80" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="135" t="s">
+      <c r="D9" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="135" t="s">
+      <c r="E9" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="69">
         <v>2010</v>
       </c>
-      <c r="G9" s="70">
+      <c r="G9" s="69">
         <v>2010</v>
       </c>
-      <c r="H9" s="127">
+      <c r="H9" s="126">
         <v>42278</v>
       </c>
-      <c r="I9" s="70" t="s">
+      <c r="I9" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="71" t="s">
+      <c r="J9" s="70" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="74"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="122"/>
-      <c r="J10" s="121"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="120"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="74"/>
-      <c r="C11" s="123" t="s">
+      <c r="B11" s="73"/>
+      <c r="C11" s="122" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="135" t="s">
+      <c r="D11" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="135" t="s">
+      <c r="E11" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="70">
+      <c r="F11" s="69">
         <v>2014</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="69">
         <v>2014</v>
       </c>
-      <c r="H11" s="127">
+      <c r="H11" s="126">
         <v>42278</v>
       </c>
-      <c r="I11" s="70" t="s">
+      <c r="I11" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="J11" s="70" t="s">
+      <c r="J11" s="69" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="74"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="74"/>
-      <c r="C13" s="149" t="s">
+      <c r="B13" s="73"/>
+      <c r="C13" s="148" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="135" t="s">
+      <c r="D13" s="134" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="135" t="s">
+      <c r="E13" s="134" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="69">
         <v>2013</v>
       </c>
-      <c r="G13" s="70">
+      <c r="G13" s="69">
         <v>2013</v>
       </c>
-      <c r="H13" s="127">
+      <c r="H13" s="126">
         <v>42278</v>
       </c>
-      <c r="I13" s="122" t="s">
+      <c r="I13" s="121" t="s">
         <v>118</v>
       </c>
-      <c r="J13" s="120" t="s">
+      <c r="J13" s="119" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="74"/>
-      <c r="C14" s="80" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="136"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
+      <c r="D14" s="135"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="74"/>
+      <c r="B15" s="73"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="74"/>
+      <c r="B16" s="73"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="74"/>
+      <c r="B17" s="73"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="74"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
     </row>
     <row r="19" spans="2:10">
-      <c r="B19" s="74"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="70"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="69"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="B20" s="74"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="70"/>
-      <c r="J20" s="70"/>
+      <c r="B20" s="73"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
     </row>
   </sheetData>
   <phoneticPr fontId="30" type="noConversion"/>
@@ -3715,1296 +3669,1290 @@
   </sheetPr>
   <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="82" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="82" customWidth="1"/>
-    <col min="3" max="3" width="9.375" style="82" customWidth="1"/>
-    <col min="4" max="4" width="4" style="82" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="82" customWidth="1"/>
-    <col min="6" max="6" width="5.25" style="82" customWidth="1"/>
-    <col min="7" max="13" width="10.625" style="82"/>
-    <col min="14" max="14" width="7.125" style="82" customWidth="1"/>
-    <col min="15" max="16384" width="10.625" style="82"/>
+    <col min="1" max="1" width="3.625" style="81" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="81" customWidth="1"/>
+    <col min="3" max="3" width="9.375" style="81" customWidth="1"/>
+    <col min="4" max="4" width="4" style="81" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="81" customWidth="1"/>
+    <col min="6" max="6" width="5.25" style="81" customWidth="1"/>
+    <col min="7" max="13" width="10.625" style="81"/>
+    <col min="14" max="14" width="7.125" style="81" customWidth="1"/>
+    <col min="15" max="16384" width="10.625" style="81"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" thickBot="1"/>
     <row r="2" spans="1:14">
-      <c r="B2" s="83"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="85"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="86"/>
-      <c r="B3" s="118"/>
-      <c r="C3" s="92" t="s">
+      <c r="A3" s="85"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="119"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="118"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="88"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="87"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="B5" s="89"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="88"/>
+      <c r="B5" s="88"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="87"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="90"/>
-      <c r="G6" s="90" t="s">
+      <c r="D6" s="89"/>
+      <c r="G6" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="88"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="87"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="88"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="87"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="87"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="89"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90">
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89">
         <v>66</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="88"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="87"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="B10" s="89"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="88"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="87"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="B11" s="89"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="87"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="B12" s="89"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="87"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="89"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90">
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89">
         <f>290*10^6</f>
         <v>290000000</v>
       </c>
-      <c r="F13" s="90" t="s">
+      <c r="F13" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="88"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="87"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="89"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="87"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90">
+      <c r="B15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89">
         <v>22</v>
       </c>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="88"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="87"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="89"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="88"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="87"/>
     </row>
     <row r="17" spans="2:14">
-      <c r="B17" s="89"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="90"/>
-      <c r="J17" s="90"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="87"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="B18" s="89"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="87"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="89"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90">
+      <c r="B19" s="88"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89">
         <v>800000000</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="90"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="88"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89"/>
+      <c r="L19" s="89"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="87"/>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="89"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="87"/>
     </row>
     <row r="21" spans="2:14">
-      <c r="B21" s="89"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="90"/>
-      <c r="J21" s="90"/>
-      <c r="K21" s="90"/>
-      <c r="L21" s="90"/>
-      <c r="M21" s="90"/>
-      <c r="N21" s="88"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="89"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="89"/>
+      <c r="N21" s="87"/>
     </row>
     <row r="22" spans="2:14">
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="90"/>
-      <c r="K22" s="90"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="90"/>
-      <c r="N22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="89"/>
+      <c r="N22" s="87"/>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="90"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="90"/>
-      <c r="N23" s="88"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="87"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="90"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="88"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="89"/>
+      <c r="N24" s="87"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="88"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="87"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="90"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="M26" s="90"/>
-      <c r="N26" s="88"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="89"/>
+      <c r="N26" s="87"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="88"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="87"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="88"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="89"/>
+      <c r="N28" s="87"/>
     </row>
     <row r="29" spans="2:14">
-      <c r="B29" s="89"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="87"/>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="90"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="90"/>
-      <c r="N30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="89"/>
+      <c r="N30" s="87"/>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="90"/>
-      <c r="J31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="89"/>
+      <c r="N31" s="87"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="90"/>
-      <c r="K32" s="90"/>
-      <c r="L32" s="90"/>
-      <c r="M32" s="90"/>
-      <c r="N32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="89"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="89"/>
+      <c r="N32" s="87"/>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="89"/>
-      <c r="C33" s="90" t="s">
+      <c r="B33" s="88"/>
+      <c r="C33" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="90">
+      <c r="D33" s="89">
         <v>128</v>
       </c>
-      <c r="E33" s="90">
+      <c r="E33" s="89">
         <v>40</v>
       </c>
-      <c r="F33" s="90" t="s">
+      <c r="F33" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="90"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="90"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="88"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="89"/>
+      <c r="J33" s="89"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="87"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="89"/>
-      <c r="G34" s="90"/>
-      <c r="H34" s="90"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="G34" s="89"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="87"/>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="89"/>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="90"/>
-      <c r="G35" s="90"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="90"/>
-      <c r="J35" s="90"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="90"/>
-      <c r="N35" s="88"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="87"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="89"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="90"/>
-      <c r="F36" s="90"/>
-      <c r="G36" s="90"/>
-      <c r="H36" s="90"/>
-      <c r="I36" s="90"/>
-      <c r="J36" s="90"/>
-      <c r="K36" s="90"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="90"/>
-      <c r="N36" s="88"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="87"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="89"/>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="90"/>
-      <c r="F37" s="90"/>
-      <c r="G37" s="90"/>
-      <c r="H37" s="124"/>
-      <c r="I37" s="90"/>
-      <c r="J37" s="90"/>
-      <c r="K37" s="90"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="90"/>
-      <c r="N37" s="88"/>
+      <c r="B37" s="88"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="123"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="89"/>
+      <c r="M37" s="89"/>
+      <c r="N37" s="87"/>
     </row>
     <row r="38" spans="2:14">
-      <c r="B38" s="89"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="90"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="90"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="90"/>
-      <c r="N38" s="88"/>
+      <c r="B38" s="88"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="87"/>
     </row>
     <row r="39" spans="2:14">
-      <c r="B39" s="89"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="90"/>
-      <c r="L39" s="90"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="88"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="89"/>
+      <c r="M39" s="89"/>
+      <c r="N39" s="87"/>
     </row>
     <row r="40" spans="2:14">
-      <c r="B40" s="89"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="90"/>
-      <c r="G40" s="90"/>
-      <c r="H40" s="90"/>
-      <c r="I40" s="90"/>
-      <c r="J40" s="90"/>
-      <c r="K40" s="90"/>
-      <c r="L40" s="90"/>
-      <c r="M40" s="90"/>
-      <c r="N40" s="88"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="89"/>
+      <c r="N40" s="87"/>
     </row>
     <row r="41" spans="2:14">
-      <c r="B41" s="89"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="90"/>
-      <c r="N41" s="88"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="89"/>
+      <c r="L41" s="89"/>
+      <c r="M41" s="89"/>
+      <c r="N41" s="87"/>
     </row>
     <row r="42" spans="2:14">
-      <c r="B42" s="89"/>
-      <c r="C42" s="90"/>
-      <c r="K42" s="90"/>
-      <c r="L42" s="90"/>
-      <c r="M42" s="90"/>
-      <c r="N42" s="88"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="89"/>
+      <c r="K42" s="89"/>
+      <c r="L42" s="89"/>
+      <c r="M42" s="89"/>
+      <c r="N42" s="87"/>
     </row>
     <row r="43" spans="2:14">
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
-      <c r="K43" s="90"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="90"/>
-      <c r="N43" s="88"/>
+      <c r="B43" s="88"/>
+      <c r="C43" s="89"/>
+      <c r="K43" s="89"/>
+      <c r="L43" s="89"/>
+      <c r="M43" s="89"/>
+      <c r="N43" s="87"/>
     </row>
     <row r="44" spans="2:14">
-      <c r="B44" s="89"/>
-      <c r="C44" s="90"/>
-      <c r="K44" s="90"/>
-      <c r="L44" s="90"/>
-      <c r="M44" s="90"/>
-      <c r="N44" s="88"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="89"/>
+      <c r="K44" s="89"/>
+      <c r="L44" s="89"/>
+      <c r="M44" s="89"/>
+      <c r="N44" s="87"/>
     </row>
     <row r="45" spans="2:14">
-      <c r="B45" s="89"/>
-      <c r="C45" s="90" t="s">
+      <c r="B45" s="88"/>
+      <c r="C45" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="K45" s="90"/>
-      <c r="L45" s="90"/>
-      <c r="M45" s="90"/>
-      <c r="N45" s="88"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="87"/>
     </row>
     <row r="46" spans="2:14">
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
-      <c r="E46" s="125">
+      <c r="B46" s="88"/>
+      <c r="C46" s="89"/>
+      <c r="E46" s="124">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
-      <c r="M46" s="90"/>
-      <c r="N46" s="88"/>
+      <c r="F46" s="89"/>
+      <c r="K46" s="89"/>
+      <c r="L46" s="89"/>
+      <c r="M46" s="89"/>
+      <c r="N46" s="87"/>
     </row>
     <row r="47" spans="2:14">
-      <c r="B47" s="89"/>
-      <c r="C47" s="90"/>
-      <c r="E47" s="90">
+      <c r="B47" s="88"/>
+      <c r="C47" s="89"/>
+      <c r="E47" s="89">
         <v>0.98499999999999999</v>
       </c>
-      <c r="F47" s="90" t="s">
+      <c r="F47" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="K47" s="90"/>
-      <c r="L47" s="90"/>
-      <c r="M47" s="90"/>
-      <c r="N47" s="88"/>
+      <c r="K47" s="89"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="89"/>
+      <c r="N47" s="87"/>
     </row>
     <row r="48" spans="2:14">
-      <c r="B48" s="89"/>
-      <c r="C48" s="90"/>
-      <c r="E48" s="82">
-        <v>1</v>
-      </c>
-      <c r="F48" s="82" t="s">
-        <v>121</v>
-      </c>
-      <c r="K48" s="90"/>
-      <c r="L48" s="90"/>
-      <c r="M48" s="90"/>
-      <c r="N48" s="88"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="89"/>
+      <c r="N48" s="87"/>
     </row>
     <row r="49" spans="2:14">
-      <c r="B49" s="89"/>
-      <c r="C49" s="90"/>
-      <c r="K49" s="90"/>
-      <c r="L49" s="90"/>
-      <c r="M49" s="90"/>
-      <c r="N49" s="88"/>
+      <c r="B49" s="88"/>
+      <c r="C49" s="89"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="89"/>
+      <c r="M49" s="89"/>
+      <c r="N49" s="87"/>
     </row>
     <row r="50" spans="2:14">
-      <c r="B50" s="89"/>
-      <c r="C50" s="90"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="90"/>
-      <c r="M50" s="90"/>
-      <c r="N50" s="88"/>
+      <c r="B50" s="88"/>
+      <c r="C50" s="89"/>
+      <c r="K50" s="89"/>
+      <c r="L50" s="89"/>
+      <c r="M50" s="89"/>
+      <c r="N50" s="87"/>
     </row>
     <row r="51" spans="2:14">
-      <c r="B51" s="89"/>
-      <c r="C51" s="90" t="s">
+      <c r="B51" s="88"/>
+      <c r="C51" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="L51" s="90"/>
-      <c r="M51" s="90"/>
-      <c r="N51" s="88"/>
+      <c r="D51" s="89"/>
+      <c r="K51" s="89"/>
+      <c r="L51" s="89"/>
+      <c r="M51" s="89"/>
+      <c r="N51" s="87"/>
     </row>
     <row r="52" spans="2:14">
-      <c r="B52" s="89"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="K52" s="90"/>
-      <c r="L52" s="90"/>
-      <c r="M52" s="90"/>
-      <c r="N52" s="88"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="K52" s="89"/>
+      <c r="L52" s="89"/>
+      <c r="M52" s="89"/>
+      <c r="N52" s="87"/>
     </row>
     <row r="53" spans="2:14">
-      <c r="B53" s="89"/>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90">
+      <c r="B53" s="88"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="89">
         <v>78</v>
       </c>
-      <c r="K53" s="90"/>
-      <c r="L53" s="90"/>
-      <c r="M53" s="90"/>
-      <c r="N53" s="88"/>
+      <c r="K53" s="89"/>
+      <c r="L53" s="89"/>
+      <c r="M53" s="89"/>
+      <c r="N53" s="87"/>
     </row>
     <row r="54" spans="2:14">
-      <c r="B54" s="89"/>
-      <c r="C54" s="90"/>
-      <c r="D54" s="90"/>
-      <c r="K54" s="90"/>
-      <c r="L54" s="90"/>
-      <c r="M54" s="90"/>
-      <c r="N54" s="88"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="89"/>
+      <c r="K54" s="89"/>
+      <c r="L54" s="89"/>
+      <c r="M54" s="89"/>
+      <c r="N54" s="87"/>
     </row>
     <row r="55" spans="2:14">
-      <c r="B55" s="89"/>
-      <c r="C55" s="90"/>
-      <c r="D55" s="90"/>
-      <c r="K55" s="90"/>
-      <c r="L55" s="90"/>
-      <c r="M55" s="90"/>
-      <c r="N55" s="88"/>
+      <c r="B55" s="88"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="89"/>
+      <c r="K55" s="89"/>
+      <c r="L55" s="89"/>
+      <c r="M55" s="89"/>
+      <c r="N55" s="87"/>
     </row>
     <row r="56" spans="2:14">
-      <c r="B56" s="89"/>
-      <c r="C56" s="90"/>
-      <c r="K56" s="90"/>
-      <c r="L56" s="90"/>
-      <c r="M56" s="90"/>
-      <c r="N56" s="88"/>
+      <c r="B56" s="88"/>
+      <c r="C56" s="89"/>
+      <c r="K56" s="89"/>
+      <c r="L56" s="89"/>
+      <c r="M56" s="89"/>
+      <c r="N56" s="87"/>
     </row>
     <row r="57" spans="2:14">
-      <c r="B57" s="89"/>
-      <c r="C57" s="90"/>
-      <c r="K57" s="90"/>
-      <c r="L57" s="90"/>
-      <c r="M57" s="90"/>
-      <c r="N57" s="88"/>
+      <c r="B57" s="88"/>
+      <c r="C57" s="89"/>
+      <c r="K57" s="89"/>
+      <c r="L57" s="89"/>
+      <c r="M57" s="89"/>
+      <c r="N57" s="87"/>
     </row>
     <row r="58" spans="2:14">
-      <c r="B58" s="89"/>
-      <c r="C58" s="90"/>
-      <c r="K58" s="90"/>
-      <c r="L58" s="90"/>
-      <c r="M58" s="90"/>
-      <c r="N58" s="88"/>
+      <c r="B58" s="88"/>
+      <c r="C58" s="89"/>
+      <c r="K58" s="89"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="87"/>
     </row>
     <row r="59" spans="2:14">
-      <c r="B59" s="89"/>
-      <c r="C59" s="90"/>
-      <c r="E59" s="82">
+      <c r="B59" s="88"/>
+      <c r="C59" s="89"/>
+      <c r="E59" s="81">
         <f>34.4925*10^6</f>
         <v>34492500</v>
       </c>
-      <c r="F59" s="82" t="s">
+      <c r="F59" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="K59" s="90"/>
-      <c r="L59" s="90"/>
-      <c r="M59" s="90"/>
-      <c r="N59" s="88"/>
+      <c r="K59" s="89"/>
+      <c r="L59" s="89"/>
+      <c r="M59" s="89"/>
+      <c r="N59" s="87"/>
     </row>
     <row r="60" spans="2:14">
-      <c r="B60" s="89"/>
-      <c r="C60" s="90"/>
-      <c r="F60" s="82">
+      <c r="B60" s="88"/>
+      <c r="C60" s="89"/>
+      <c r="F60" s="81">
         <v>1.0833999999999999</v>
       </c>
-      <c r="G60" s="82" t="s">
+      <c r="G60" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="K60" s="90"/>
-      <c r="L60" s="90"/>
-      <c r="M60" s="90"/>
-      <c r="N60" s="88"/>
+      <c r="K60" s="89"/>
+      <c r="L60" s="89"/>
+      <c r="M60" s="89"/>
+      <c r="N60" s="87"/>
     </row>
     <row r="61" spans="2:14">
-      <c r="B61" s="89"/>
-      <c r="C61" s="90"/>
-      <c r="K61" s="90"/>
-      <c r="L61" s="90"/>
-      <c r="M61" s="90"/>
-      <c r="N61" s="88"/>
+      <c r="B61" s="88"/>
+      <c r="C61" s="89"/>
+      <c r="K61" s="89"/>
+      <c r="L61" s="89"/>
+      <c r="M61" s="89"/>
+      <c r="N61" s="87"/>
     </row>
     <row r="62" spans="2:14">
-      <c r="B62" s="89"/>
-      <c r="C62" s="90"/>
-      <c r="F62" s="82" t="s">
+      <c r="B62" s="88"/>
+      <c r="C62" s="89"/>
+      <c r="F62" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="K62" s="90"/>
-      <c r="L62" s="90"/>
-      <c r="M62" s="90"/>
-      <c r="N62" s="88"/>
+      <c r="K62" s="89"/>
+      <c r="L62" s="89"/>
+      <c r="M62" s="89"/>
+      <c r="N62" s="87"/>
     </row>
     <row r="63" spans="2:14">
-      <c r="B63" s="89"/>
-      <c r="C63" s="90"/>
-      <c r="F63" s="82">
+      <c r="B63" s="88"/>
+      <c r="C63" s="89"/>
+      <c r="F63" s="81">
         <v>16</v>
       </c>
-      <c r="G63" s="82" t="s">
+      <c r="G63" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="K63" s="90"/>
-      <c r="L63" s="90"/>
-      <c r="M63" s="90"/>
-      <c r="N63" s="88"/>
+      <c r="K63" s="89"/>
+      <c r="L63" s="89"/>
+      <c r="M63" s="89"/>
+      <c r="N63" s="87"/>
     </row>
     <row r="64" spans="2:14">
-      <c r="B64" s="89"/>
-      <c r="C64" s="90"/>
-      <c r="F64" s="82">
+      <c r="B64" s="88"/>
+      <c r="C64" s="89"/>
+      <c r="F64" s="81">
         <f>16000000000*0.833</f>
         <v>13328000000</v>
       </c>
-      <c r="G64" s="82" t="s">
+      <c r="G64" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="H64" s="82" t="s">
+      <c r="H64" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="K64" s="90"/>
-      <c r="L64" s="90"/>
-      <c r="M64" s="90"/>
-      <c r="N64" s="88"/>
+      <c r="K64" s="89"/>
+      <c r="L64" s="89"/>
+      <c r="M64" s="89"/>
+      <c r="N64" s="87"/>
     </row>
     <row r="65" spans="2:14">
-      <c r="B65" s="89"/>
-      <c r="C65" s="90"/>
-      <c r="F65" s="82">
+      <c r="B65" s="88"/>
+      <c r="C65" s="89"/>
+      <c r="F65" s="81">
         <f>F64*38.018--7203</f>
         <v>506703911203</v>
       </c>
-      <c r="G65" s="82" t="s">
+      <c r="G65" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="K65" s="90"/>
-      <c r="L65" s="90"/>
-      <c r="M65" s="90"/>
-      <c r="N65" s="88"/>
+      <c r="K65" s="89"/>
+      <c r="L65" s="89"/>
+      <c r="M65" s="89"/>
+      <c r="N65" s="87"/>
     </row>
     <row r="66" spans="2:14">
-      <c r="B66" s="89"/>
-      <c r="C66" s="90"/>
-      <c r="F66" s="82">
+      <c r="B66" s="88"/>
+      <c r="C66" s="89"/>
+      <c r="F66" s="81">
         <f>F65/(10^9)</f>
         <v>506.70391120300002</v>
       </c>
-      <c r="G66" s="82" t="s">
+      <c r="G66" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="K66" s="90"/>
-      <c r="L66" s="90"/>
-      <c r="M66" s="90"/>
-      <c r="N66" s="88"/>
+      <c r="K66" s="89"/>
+      <c r="L66" s="89"/>
+      <c r="M66" s="89"/>
+      <c r="N66" s="87"/>
     </row>
     <row r="67" spans="2:14">
-      <c r="B67" s="89"/>
-      <c r="C67" s="90"/>
-      <c r="F67" s="82">
+      <c r="B67" s="88"/>
+      <c r="C67" s="89"/>
+      <c r="F67" s="81">
         <f>F66/365</f>
         <v>1.3882298937068493</v>
       </c>
-      <c r="G67" s="82" t="s">
+      <c r="G67" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="K67" s="90"/>
-      <c r="L67" s="90"/>
-      <c r="M67" s="90"/>
-      <c r="N67" s="88"/>
+      <c r="K67" s="89"/>
+      <c r="L67" s="89"/>
+      <c r="M67" s="89"/>
+      <c r="N67" s="87"/>
     </row>
     <row r="68" spans="2:14">
-      <c r="B68" s="89"/>
-      <c r="C68" s="90"/>
-      <c r="K68" s="90"/>
-      <c r="L68" s="90"/>
-      <c r="M68" s="90"/>
-      <c r="N68" s="88"/>
+      <c r="B68" s="88"/>
+      <c r="C68" s="89"/>
+      <c r="K68" s="89"/>
+      <c r="L68" s="89"/>
+      <c r="M68" s="89"/>
+      <c r="N68" s="87"/>
     </row>
     <row r="69" spans="2:14">
-      <c r="B69" s="89"/>
-      <c r="C69" s="90"/>
-      <c r="F69" s="82" t="s">
+      <c r="B69" s="88"/>
+      <c r="C69" s="89"/>
+      <c r="F69" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="K69" s="90"/>
-      <c r="L69" s="90"/>
-      <c r="M69" s="90"/>
-      <c r="N69" s="88"/>
+      <c r="K69" s="89"/>
+      <c r="L69" s="89"/>
+      <c r="M69" s="89"/>
+      <c r="N69" s="87"/>
     </row>
     <row r="70" spans="2:14">
-      <c r="B70" s="89"/>
-      <c r="C70" s="90" t="s">
+      <c r="B70" s="88"/>
+      <c r="C70" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="K70" s="90"/>
-      <c r="L70" s="90"/>
-      <c r="M70" s="90"/>
-      <c r="N70" s="88"/>
+      <c r="K70" s="89"/>
+      <c r="L70" s="89"/>
+      <c r="M70" s="89"/>
+      <c r="N70" s="87"/>
     </row>
     <row r="71" spans="2:14">
-      <c r="B71" s="89"/>
-      <c r="C71" s="90"/>
-      <c r="D71" s="82">
+      <c r="B71" s="88"/>
+      <c r="C71" s="89"/>
+      <c r="D71" s="81">
         <v>70</v>
       </c>
-      <c r="E71" s="82">
+      <c r="E71" s="81">
         <f>E59*F67/F60</f>
         <v>44197452.103270732</v>
       </c>
-      <c r="F71" s="82" t="s">
+      <c r="F71" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="K71" s="90"/>
-      <c r="L71" s="90"/>
-      <c r="M71" s="90"/>
-      <c r="N71" s="88"/>
+      <c r="K71" s="89"/>
+      <c r="L71" s="89"/>
+      <c r="M71" s="89"/>
+      <c r="N71" s="87"/>
     </row>
     <row r="72" spans="2:14">
-      <c r="B72" s="89"/>
-      <c r="C72" s="90"/>
-      <c r="E72" s="82">
+      <c r="B72" s="88"/>
+      <c r="C72" s="89"/>
+      <c r="E72" s="81">
         <f>Exchange_rates!E9</f>
         <v>1.0980000000000001</v>
       </c>
-      <c r="F72" s="82" t="s">
+      <c r="F72" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="K72" s="90"/>
-      <c r="L72" s="90"/>
-      <c r="M72" s="90"/>
-      <c r="N72" s="88"/>
+      <c r="K72" s="89"/>
+      <c r="L72" s="89"/>
+      <c r="M72" s="89"/>
+      <c r="N72" s="87"/>
     </row>
     <row r="73" spans="2:14">
-      <c r="B73" s="89"/>
-      <c r="C73" s="90"/>
-      <c r="E73" s="82">
+      <c r="B73" s="88"/>
+      <c r="C73" s="89"/>
+      <c r="E73" s="81">
         <f>E71/E72</f>
         <v>40252688.618643649</v>
       </c>
-      <c r="F73" s="82" t="s">
+      <c r="F73" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="K73" s="90"/>
-      <c r="L73" s="90"/>
-      <c r="M73" s="90"/>
-      <c r="N73" s="88"/>
+      <c r="K73" s="89"/>
+      <c r="L73" s="89"/>
+      <c r="M73" s="89"/>
+      <c r="N73" s="87"/>
     </row>
     <row r="74" spans="2:14">
-      <c r="B74" s="89"/>
-      <c r="K74" s="90"/>
-      <c r="L74" s="90"/>
-      <c r="M74" s="90"/>
-      <c r="N74" s="88"/>
+      <c r="B74" s="88"/>
+      <c r="K74" s="89"/>
+      <c r="L74" s="89"/>
+      <c r="M74" s="89"/>
+      <c r="N74" s="87"/>
     </row>
     <row r="75" spans="2:14">
-      <c r="B75" s="89"/>
-      <c r="K75" s="90"/>
-      <c r="L75" s="90"/>
-      <c r="M75" s="90"/>
-      <c r="N75" s="88"/>
+      <c r="B75" s="88"/>
+      <c r="K75" s="89"/>
+      <c r="L75" s="89"/>
+      <c r="M75" s="89"/>
+      <c r="N75" s="87"/>
     </row>
     <row r="76" spans="2:14">
-      <c r="B76" s="89"/>
+      <c r="B76" s="88"/>
     </row>
     <row r="77" spans="2:14">
-      <c r="B77" s="89"/>
-      <c r="E77" s="82">
+      <c r="B77" s="88"/>
+      <c r="E77" s="81">
         <v>0.12364799999999999</v>
       </c>
-      <c r="F77" s="82" t="s">
+      <c r="F77" s="81" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="78" spans="2:14">
-      <c r="B78" s="89"/>
-      <c r="E78" s="82">
+      <c r="B78" s="88"/>
+      <c r="E78" s="81">
         <f>E77/1000</f>
         <v>1.2364799999999999E-4</v>
       </c>
-      <c r="F78" s="82" t="s">
+      <c r="F78" s="81" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="79" spans="2:14">
-      <c r="B79" s="89"/>
-      <c r="C79" s="90"/>
-      <c r="E79" s="82">
+      <c r="B79" s="88"/>
+      <c r="C79" s="89"/>
+      <c r="E79" s="81">
         <f>Exchange_rates!E9</f>
         <v>1.0980000000000001</v>
       </c>
-      <c r="F79" s="82" t="s">
+      <c r="F79" s="81" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="80" spans="2:14">
-      <c r="B80" s="89"/>
-      <c r="C80" s="90"/>
-      <c r="D80" s="90"/>
-      <c r="E80" s="82">
+      <c r="B80" s="88"/>
+      <c r="C80" s="89"/>
+      <c r="D80" s="89"/>
+      <c r="E80" s="81">
         <f>E78/E79</f>
         <v>1.1261202185792348E-4</v>
       </c>
-      <c r="F80" s="82" t="s">
+      <c r="F80" s="81" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="81" spans="2:3">
-      <c r="B81" s="89"/>
-      <c r="C81" s="90"/>
+      <c r="B81" s="88"/>
+      <c r="C81" s="89"/>
     </row>
     <row r="82" spans="2:3">
-      <c r="B82" s="89"/>
+      <c r="B82" s="88"/>
     </row>
     <row r="83" spans="2:3">
-      <c r="B83" s="89"/>
+      <c r="B83" s="88"/>
     </row>
     <row r="84" spans="2:3">
-      <c r="B84" s="89"/>
+      <c r="B84" s="88"/>
     </row>
     <row r="85" spans="2:3">
-      <c r="B85" s="89"/>
+      <c r="B85" s="88"/>
     </row>
     <row r="86" spans="2:3">
-      <c r="B86" s="89"/>
+      <c r="B86" s="88"/>
     </row>
     <row r="87" spans="2:3">
-      <c r="B87" s="89"/>
+      <c r="B87" s="88"/>
     </row>
     <row r="88" spans="2:3">
-      <c r="B88" s="89"/>
+      <c r="B88" s="88"/>
     </row>
     <row r="89" spans="2:3">
-      <c r="B89" s="89"/>
+      <c r="B89" s="88"/>
     </row>
     <row r="90" spans="2:3">
-      <c r="B90" s="89"/>
+      <c r="B90" s="88"/>
     </row>
     <row r="91" spans="2:3">
-      <c r="B91" s="89"/>
+      <c r="B91" s="88"/>
     </row>
     <row r="92" spans="2:3">
-      <c r="B92" s="89"/>
-      <c r="C92" s="90"/>
+      <c r="B92" s="88"/>
+      <c r="C92" s="89"/>
     </row>
     <row r="93" spans="2:3">
-      <c r="B93" s="89"/>
-      <c r="C93" s="90"/>
+      <c r="B93" s="88"/>
+      <c r="C93" s="89"/>
     </row>
     <row r="94" spans="2:3">
-      <c r="B94" s="89"/>
-      <c r="C94" s="90"/>
+      <c r="B94" s="88"/>
+      <c r="C94" s="89"/>
     </row>
     <row r="95" spans="2:3">
-      <c r="B95" s="89"/>
-      <c r="C95" s="90"/>
+      <c r="B95" s="88"/>
+      <c r="C95" s="89"/>
     </row>
     <row r="96" spans="2:3">
-      <c r="B96" s="89"/>
-      <c r="C96" s="90"/>
+      <c r="B96" s="88"/>
+      <c r="C96" s="89"/>
     </row>
     <row r="97" spans="2:3">
-      <c r="B97" s="89"/>
-      <c r="C97" s="90"/>
+      <c r="B97" s="88"/>
+      <c r="C97" s="89"/>
     </row>
     <row r="98" spans="2:3">
-      <c r="B98" s="89"/>
+      <c r="B98" s="88"/>
     </row>
     <row r="99" spans="2:3">
-      <c r="B99" s="89"/>
+      <c r="B99" s="88"/>
     </row>
     <row r="100" spans="2:3">
-      <c r="B100" s="89"/>
+      <c r="B100" s="88"/>
     </row>
     <row r="101" spans="2:3">
-      <c r="B101" s="89"/>
+      <c r="B101" s="88"/>
     </row>
     <row r="102" spans="2:3">
-      <c r="B102" s="89"/>
+      <c r="B102" s="88"/>
     </row>
     <row r="103" spans="2:3">
-      <c r="B103" s="89"/>
+      <c r="B103" s="88"/>
     </row>
     <row r="104" spans="2:3">
-      <c r="B104" s="89"/>
+      <c r="B104" s="88"/>
     </row>
     <row r="105" spans="2:3">
-      <c r="B105" s="89"/>
+      <c r="B105" s="88"/>
     </row>
     <row r="106" spans="2:3">
-      <c r="B106" s="89"/>
+      <c r="B106" s="88"/>
     </row>
     <row r="107" spans="2:3">
-      <c r="B107" s="89"/>
+      <c r="B107" s="88"/>
     </row>
     <row r="108" spans="2:3">
-      <c r="B108" s="89"/>
+      <c r="B108" s="88"/>
     </row>
     <row r="109" spans="2:3">
-      <c r="B109" s="89"/>
+      <c r="B109" s="88"/>
     </row>
     <row r="110" spans="2:3">
-      <c r="B110" s="89"/>
+      <c r="B110" s="88"/>
     </row>
     <row r="111" spans="2:3">
-      <c r="B111" s="89"/>
+      <c r="B111" s="88"/>
     </row>
     <row r="112" spans="2:3">
-      <c r="B112" s="89"/>
+      <c r="B112" s="88"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="89"/>
+      <c r="B113" s="88"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="89"/>
+      <c r="B114" s="88"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="89"/>
+      <c r="B115" s="88"/>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="89"/>
+      <c r="B116" s="88"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="89"/>
+      <c r="B117" s="88"/>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="89"/>
+      <c r="B118" s="88"/>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="89"/>
+      <c r="B119" s="88"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="89"/>
+      <c r="B120" s="88"/>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="89"/>
+      <c r="B121" s="88"/>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="89"/>
+      <c r="B122" s="88"/>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="89"/>
+      <c r="B123" s="88"/>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="89"/>
+      <c r="B124" s="88"/>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="89"/>
+      <c r="B125" s="88"/>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="89"/>
+      <c r="B126" s="88"/>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="89"/>
+      <c r="B127" s="88"/>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="89"/>
+      <c r="B128" s="88"/>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="89"/>
+      <c r="B129" s="88"/>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="89"/>
+      <c r="B130" s="88"/>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="89"/>
+      <c r="B131" s="88"/>
     </row>
     <row r="132" spans="2:2">
-      <c r="B132" s="89"/>
+      <c r="B132" s="88"/>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="89"/>
+      <c r="B133" s="88"/>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="89"/>
+      <c r="B134" s="88"/>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="89"/>
+      <c r="B135" s="88"/>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="89"/>
+      <c r="B136" s="88"/>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="89"/>
+      <c r="B137" s="88"/>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="89"/>
+      <c r="B138" s="88"/>
     </row>
     <row r="139" spans="2:2">
-      <c r="B139" s="89"/>
+      <c r="B139" s="88"/>
     </row>
     <row r="140" spans="2:2">
-      <c r="B140" s="89"/>
+      <c r="B140" s="88"/>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="89"/>
+      <c r="B141" s="88"/>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="89"/>
+      <c r="B142" s="88"/>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="89"/>
+      <c r="B143" s="88"/>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="89"/>
+      <c r="B144" s="88"/>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="89"/>
+      <c r="B145" s="88"/>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="89"/>
+      <c r="B146" s="88"/>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="89"/>
+      <c r="B147" s="88"/>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="89"/>
+      <c r="B148" s="88"/>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="89"/>
+      <c r="B149" s="88"/>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="89"/>
+      <c r="B150" s="88"/>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="89"/>
+      <c r="B151" s="88"/>
     </row>
     <row r="152" spans="2:2">
-      <c r="B152" s="89"/>
+      <c r="B152" s="88"/>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="89"/>
+      <c r="B153" s="88"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5036,80 +4984,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="136"/>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
+      <c r="A1" s="135"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="136"/>
+      <c r="A2" s="135"/>
       <c r="B2" s="154" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="155"/>
       <c r="D2" s="155"/>
       <c r="E2" s="163"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="136"/>
+      <c r="A3" s="135"/>
       <c r="B3" s="157"/>
       <c r="C3" s="158"/>
       <c r="D3" s="158"/>
       <c r="E3" s="164"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="136"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="160"/>
       <c r="C4" s="161"/>
       <c r="D4" s="161"/>
       <c r="E4" s="165"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
     </row>
     <row r="5" spans="1:9" ht="17" thickBot="1">
-      <c r="A5" s="136"/>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
+      <c r="A5" s="135"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="136"/>
-      <c r="B6" s="138"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="139"/>
+      <c r="I6" s="138"/>
     </row>
     <row r="7" spans="1:9" ht="18">
-      <c r="A7" s="140"/>
-      <c r="B7" s="141"/>
+      <c r="A7" s="139"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="142" t="s">
+      <c r="D7" s="141" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -5124,34 +5072,34 @@
       <c r="H7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="143"/>
+      <c r="I7" s="142"/>
     </row>
     <row r="8" spans="1:9" ht="19" thickBot="1">
       <c r="B8" s="25"/>
-      <c r="I8" s="144"/>
+      <c r="I8" s="143"/>
     </row>
     <row r="9" spans="1:9" ht="19" thickBot="1">
-      <c r="A9" s="140"/>
+      <c r="A9" s="139"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="145" t="s">
+      <c r="C9" s="144" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="146">
+      <c r="E9" s="145">
         <v>1.0980000000000001</v>
       </c>
-      <c r="F9" s="145" t="s">
+      <c r="F9" s="144" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="147">
+      <c r="G9" s="146">
         <v>42221</v>
       </c>
-      <c r="H9" s="148" t="s">
+      <c r="H9" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="144"/>
+      <c r="I9" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>